<commit_message>
Entregables actualizados / historias de  usuario, RF RNF
</commit_message>
<xml_diff>
--- a/entregables/EscalaDeValoracion.xlsx
+++ b/entregables/EscalaDeValoracion.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="442" documentId="11_7E4E55BF84DCCEE3ED7FF6F99031F45BFA722949" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{927AB1BB-534A-493F-8246-13B12934B54B}"/>
+  <xr:revisionPtr revIDLastSave="445" documentId="11_7E4E55BF84DCCEE3ED7FF6F99031F45BFA722949" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35BEF066-797F-4EE5-AB4B-FE2EDEBF1671}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Escala" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>PREGUNTAS</t>
   </si>
@@ -49,64 +49,61 @@
     <t>Gestión de ventas</t>
   </si>
   <si>
+    <t>¿Qué estrategias se implementan para retener a los clientes?</t>
+  </si>
+  <si>
+    <t>Ninguna</t>
+  </si>
+  <si>
+    <t>¿Qué tan eficiente es el proceso de registro y seguimiento de las ventas?</t>
+  </si>
+  <si>
+    <t>¿Qué medidas se toman para garantizar un ambiente de trabajo positivo y seguro?</t>
+  </si>
+  <si>
+    <t>Tratamos de mantener una relación más que un jefe un amigo, sacamos espacios para compartir fuera del lugar de trabajo.</t>
+  </si>
+  <si>
+    <t>¿Qué tan rápido y eficiente es el proceso de atención al cliente y toma de pedidos?</t>
+  </si>
+  <si>
+    <t>¿Qué tipos de informes se generan para analizar las ventas?</t>
+  </si>
+  <si>
+    <t>Ninguno</t>
+  </si>
+  <si>
+    <t>¿Qué tan efectivas son las estrategias para aumentar las ventas?</t>
+  </si>
+  <si>
+    <t>¿Qué tan bien se manejan las quejas o problemas de los clientes?</t>
+  </si>
+  <si>
+    <t>Gestión de inventario</t>
+  </si>
+  <si>
+    <t>¿Qué tan preciso es el control de inventario?</t>
+  </si>
+  <si>
+    <t>¿Se minimiza eficazmente el desperdicio de alimentos?</t>
+  </si>
+  <si>
+    <t>¿Se lleva un registro de las fechas de vencimiento de los productos perecederos?</t>
+  </si>
+  <si>
+    <t>Facturación</t>
+  </si>
+  <si>
+    <t>¿Qué tan rápido se emiten las facturas después de realizar un pedido?</t>
+  </si>
+  <si>
+    <t>¿Se ofrecen múltiples opciones de pago para los clientes?</t>
+  </si>
+  <si>
+    <t>¿Qué tan precisas son las facturas emitidas?</t>
+  </si>
+  <si>
     <t>¿Cómo se manejan las disputas o errores en las facturas?</t>
-  </si>
-  <si>
-    <t>El sistema permite que el administrador eliminé o modifique facturas ya hechas con alguna anotación y observación.</t>
-  </si>
-  <si>
-    <t>¿Qué tan eficiente es el proceso de registro y seguimiento de las ventas?</t>
-  </si>
-  <si>
-    <t>¿Qué estrategias se implementan para retener a los clientes?</t>
-  </si>
-  <si>
-    <t>Ninguna</t>
-  </si>
-  <si>
-    <t>¿Qué tan rápido y eficiente es el proceso de atención al cliente y toma de pedidos?</t>
-  </si>
-  <si>
-    <t>¿Qué medidas se toman para garantizar un ambiente de trabajo positivo y seguro?</t>
-  </si>
-  <si>
-    <t>Tratamos de mantener una relación más que un jefe un amigo, sacamos espacios para compartir fuera del lugar de trabajo.</t>
-  </si>
-  <si>
-    <t>¿Qué tan efectivas son las estrategias para aumentar las ventas?</t>
-  </si>
-  <si>
-    <t>¿Qué tipos de informes se generan para analizar las ventas?</t>
-  </si>
-  <si>
-    <t>El programa muestra un informe mensual o semanal según lo modifique</t>
-  </si>
-  <si>
-    <t>¿Qué tan bien se manejan las quejas o problemas de los clientes?</t>
-  </si>
-  <si>
-    <t>Gestión de inventario</t>
-  </si>
-  <si>
-    <t>¿Qué tan preciso es el control de inventario?</t>
-  </si>
-  <si>
-    <t>¿Se minimiza eficazmente el desperdicio de alimentos?</t>
-  </si>
-  <si>
-    <t>¿Se lleva un registro de las fechas de vencimiento de los productos perecederos?</t>
-  </si>
-  <si>
-    <t>Facturación</t>
-  </si>
-  <si>
-    <t>¿Qué tan rápido se emiten las facturas después de realizar un pedido?</t>
-  </si>
-  <si>
-    <t>¿Se ofrecen múltiples opciones de pago para los clientes?</t>
-  </si>
-  <si>
-    <t>¿Qué tan precisas son las facturas emitidas?</t>
   </si>
   <si>
     <t>Fidelización</t>
@@ -308,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -316,13 +313,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -348,31 +339,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,12 +361,31 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1641,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0235E6F5-E368-46FF-9E39-378C9C8243B3}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1662,10 +1657,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
@@ -1678,10 +1673,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="1"/>
       <c r="E3" s="2" t="s">
         <v>5</v>
@@ -1692,7 +1687,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2">
@@ -1708,10 +1703,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
       <c r="D5" s="1"/>
@@ -1724,26 +1719,20 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1"/>
-      <c r="B7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" s="1"/>
@@ -1751,17 +1740,17 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1"/>
-      <c r="B8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="14"/>
+      <c r="B8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="24"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1"/>
-      <c r="B9" s="9" t="s">
-        <v>18</v>
+      <c r="B9" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1771,10 +1760,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
-      <c r="B10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3">
         <v>2</v>
       </c>
       <c r="D10" s="1"/>
@@ -1782,8 +1771,8 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>
-      <c r="B11" s="9" t="s">
-        <v>20</v>
+      <c r="B11" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C11" s="2">
         <v>4</v>
@@ -1793,17 +1782,17 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1"/>
-      <c r="B12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="14"/>
+      <c r="B12" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="24"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1"/>
-      <c r="B13" s="9" t="s">
-        <v>22</v>
+      <c r="B13" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
@@ -1813,10 +1802,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1"/>
-      <c r="B14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3">
         <v>5</v>
       </c>
       <c r="D14" s="1"/>
@@ -1824,8 +1813,8 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1"/>
-      <c r="B15" s="9" t="s">
-        <v>24</v>
+      <c r="B15" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C15" s="2">
         <v>4</v>
@@ -1835,10 +1824,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1"/>
-      <c r="B16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="B16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
         <v>3</v>
       </c>
       <c r="D16" s="1"/>
@@ -1846,17 +1835,17 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
-      <c r="B17" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="14"/>
+      <c r="B17" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="24"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1"/>
-      <c r="B18" s="9" t="s">
-        <v>26</v>
+      <c r="B18" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
@@ -1866,10 +1855,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
-      <c r="B19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3">
         <v>4</v>
       </c>
       <c r="D19" s="1"/>
@@ -1877,8 +1866,8 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
-      <c r="B20" s="9" t="s">
-        <v>28</v>
+      <c r="B20" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -1888,17 +1877,17 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
-      <c r="B21" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="16"/>
+      <c r="B21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="12"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1"/>
-      <c r="B22" s="9" t="s">
-        <v>30</v>
+      <c r="B22" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C22" s="2">
         <v>3</v>
@@ -1908,10 +1897,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1"/>
-      <c r="B23" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3">
         <v>4</v>
       </c>
       <c r="D23" s="1"/>
@@ -1919,17 +1908,17 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1"/>
-      <c r="B24" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="16"/>
+      <c r="B24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="12"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1"/>
-      <c r="B25" s="9" t="s">
-        <v>33</v>
+      <c r="B25" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C25" s="2">
         <v>3</v>
@@ -1939,10 +1928,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>
-      <c r="B26" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="4">
+      <c r="B26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3">
         <v>2</v>
       </c>
       <c r="D26" s="1"/>
@@ -1957,38 +1946,38 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
-      <c r="B28" s="6" t="s">
-        <v>35</v>
+      <c r="B28" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
-      <c r="B29" s="6" t="s">
-        <v>36</v>
+      <c r="B29" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="B31" s="6" t="s">
+    <row r="32" spans="1:5">
+      <c r="B32" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="B32" s="6" t="s">
+    <row r="33" spans="2:2">
+      <c r="B33" s="4" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2006,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8FEEE5-756B-46B7-87A3-DC2057FBB735}">
   <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2027,279 +2016,269 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="15.75">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="H2" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="21"/>
-      <c r="K2" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="21"/>
-      <c r="N2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="5"/>
-      <c r="Q2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="5"/>
+      <c r="C2" s="25"/>
+      <c r="E2" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="H2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="29"/>
+      <c r="K2" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="29"/>
+      <c r="N2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="27"/>
+      <c r="Q2" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="27"/>
     </row>
     <row r="3" spans="2:18">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="18" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="4" spans="2:18">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>18</v>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>22</v>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="I4" s="2">
         <v>4</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>26</v>
+      <c r="K4" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="L4" s="2">
         <v>2</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>30</v>
+      <c r="N4" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="O4" s="2">
         <v>3</v>
       </c>
-      <c r="Q4" s="9" t="s">
-        <v>33</v>
+      <c r="Q4" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="R4" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:18">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="H5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="3">
         <v>5</v>
       </c>
-      <c r="K5" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="25">
+      <c r="K5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="18">
         <v>4</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5" s="4">
+      <c r="N5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="3">
         <v>4</v>
       </c>
-      <c r="Q5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="4">
+      <c r="Q5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:18">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>20</v>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F6" s="2">
         <v>4</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>24</v>
+      <c r="H6" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="I6" s="2">
         <v>4</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>28</v>
+      <c r="K6" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="L6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:18">
-      <c r="B7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="H7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="3">
         <v>3</v>
       </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="23"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="9" spans="2:18">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="29"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="21"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="21"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="8" t="str">
+      <c r="B10" s="6" t="str">
         <f>B2</f>
         <v>Gestión de ventas</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <f>AVERAGE(C4:C7)</f>
         <v>2.75</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
     </row>
     <row r="11" spans="2:18">
-      <c r="B11" s="8" t="str">
+      <c r="B11" s="6" t="str">
         <f>E2</f>
         <v>Gestión de inventario</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="22">
         <f>AVERAGE(F4:F6)</f>
         <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="12" spans="2:18">
-      <c r="B12" s="8" t="str">
+      <c r="B12" s="6" t="str">
         <f>H2</f>
         <v>Facturación</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <f>AVERAGE(I4:I7)</f>
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:18">
-      <c r="B13" s="8" t="str">
+      <c r="B13" s="6" t="str">
         <f>K2</f>
         <v>Fidelización</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="22">
         <f>AVERAGE(L4:L6)</f>
         <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="14" spans="2:18">
-      <c r="B14" s="8" t="str">
+      <c r="B14" s="6" t="str">
         <f>N2</f>
         <v>Administración de empleados</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="22">
         <f>AVERAGE(O4:O5)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="15" spans="2:18">
-      <c r="B15" s="8" t="str">
+      <c r="B15" s="6" t="str">
         <f>Q2</f>
         <v>Generación de informes de ventas</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="22">
         <f>AVERAGE(R4:R5)</f>
         <v>2.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="Q2:R2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>